<commit_message>
Just new Test Case msh aktr
</commit_message>
<xml_diff>
--- a/sample_constraints.xlsx
+++ b/sample_constraints.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8610590cbf95aee3/Desktop/Darsh/thesis-scheduler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="11_F25DC773A252ABDACC104824611C5F9A5BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75DEB0AD-CAC8-4B20-85A6-7AB6A01D4DD1}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="11_F25DC773A252ABDACC104824611C5F9A5BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9251B082-49BA-4AB4-9A45-86E4D6914E04}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Name</t>
   </si>
@@ -36,10 +36,10 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Dr. Amr</t>
+    <t>Reviewer 1</t>
   </si>
   <si>
-    <t>amr@guc.edu.eg</t>
+    <t>rev1@example.com</t>
   </si>
 </sst>
 </file>
@@ -112,10 +112,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -384,7 +380,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -409,7 +405,7 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3">
@@ -417,15 +413,9 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3">
-        <v>45902</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>